<commit_message>
Add Switch Mount pin symbol
</commit_message>
<xml_diff>
--- a/fab/Hotp4ck60-bottom-pos.xlsx
+++ b/fab/Hotp4ck60-bottom-pos.xlsx
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="J109" sqref="J108:J109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3679,10 +3679,10 @@
         <v>163</v>
       </c>
       <c r="D120">
-        <v>188.24</v>
+        <v>186.85</v>
       </c>
       <c r="E120">
-        <v>-164.31</v>
+        <v>-162.61000000000001</v>
       </c>
       <c r="F120">
         <v>180</v>

</xml_diff>